<commit_message>
fix to ig profile dataentry and profile excel import test file;
git-svn-id: https://svn.fao.org/projects/ruralinvest/RIV4/trunk@66763 d7fa552c-c32d-11e1-9f2d-6d39f2a56844
</commit_message>
<xml_diff>
--- a/RIV4-tests/src/test/resources/imports/profile/product.xlsx
+++ b/RIV4-tests/src/test/resources/imports/profile/product.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Product One</t>
   </si>
@@ -88,10 +88,6 @@
   </si>
   <si>
     <t>p/day</t>
-  </si>
-  <si>
-    <t>foo</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -479,7 +475,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -591,8 +587,8 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>23</v>
+      <c r="A10">
+        <v>0</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -601,7 +597,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E10" s="3">
         <v>0</v>
@@ -712,6 +708,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
improvement to profileexcelimport test; fix for profile product excel import file;
git-svn-id: https://svn.fao.org/projects/ruralinvest/RIV4/trunk@66764 d7fa552c-c32d-11e1-9f2d-6d39f2a56844
</commit_message>
<xml_diff>
--- a/RIV4-tests/src/test/resources/imports/profile/product.xlsx
+++ b/RIV4-tests/src/test/resources/imports/profile/product.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="130404" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>Product One</t>
   </si>
@@ -475,7 +475,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -587,8 +587,8 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10">
-        <v>0</v>
+      <c r="A10" t="s">
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -711,6 +711,7 @@
   <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>